<commit_message>
Test Case added 29/05/2019
</commit_message>
<xml_diff>
--- a/Test Case/Rijo/Test Case - Nursing Station.xlsx
+++ b/Test Case/Rijo/Test Case - Nursing Station.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Mediware\CentralRepository-Mediware\Test Case\Rijo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Mediware\CentralRepository-Mediware\Test Case\Rijo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE3D445-343B-4D8F-8DD8-728598C4000F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AFA7D8-1106-4214-9B19-9B294C07F791}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,11 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="187">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -347,7 +340,304 @@
 Loose:</t>
   </si>
   <si>
-    <t>Materials should be record in the Issued  To Patient section</t>
+    <t>MED_NURS_TC_011</t>
+  </si>
+  <si>
+    <t>Materials should be recorded in the Issued  To Patient section</t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursing Notes&gt;&gt;Vital Signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vital Sign entry form should be displayed </t>
+  </si>
+  <si>
+    <t>Verify that a nurse is able to add Vital Signs for the current time and date</t>
+  </si>
+  <si>
+    <t>Vital Sign should be saved successfully</t>
+  </si>
+  <si>
+    <t>Temp:
+Pulse:
+Resp:
+BP:
+Weight
+Height:
+BMI:
+SPO2:</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_012</t>
+  </si>
+  <si>
+    <t>Verify that a nurse is able to add Vital Signs for a specified time and date</t>
+  </si>
+  <si>
+    <t>Click the checkbox Change Date &amp; Time and enter the vital sign</t>
+  </si>
+  <si>
+    <t>Enter the vital sign</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that a nurse is able to add nursing notes for the patient </t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursing Notes&gt;&gt;Nursing Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nursing notes entry page should be displayed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entry date and time should be selected </t>
+  </si>
+  <si>
+    <t>Add nursing notes and plan of action. Save the notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nursing notes should be saved </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the date and time form the date picker. Check the box if "Precaution Alert" is need </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that a nurse is not able to add nursing notes for the patient in future date </t>
+  </si>
+  <si>
+    <t>Add nursing notes and plan of action for a future date. Save the notes</t>
+  </si>
+  <si>
+    <t>Nursing notes should not be saved. It should display the message "Nursing notes entry is blocked for future date"</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_014</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_015</t>
+  </si>
+  <si>
+    <t>Verify whether a nurse can enter Infusion/Transfusion details</t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursing Notes&gt;&gt;Infusion/Transfusion Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nursing notes entry page should be displayed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infusion/Transfusion entry page should be displayed </t>
+  </si>
+  <si>
+    <t>Select the start date for Infusion/Transfusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start date should be selected </t>
+  </si>
+  <si>
+    <t>Item:
+Qty(ml):
+Remarks:</t>
+  </si>
+  <si>
+    <t>Infusion/Transfusion details should be entered and saved  successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Infusion/Transfusion details. Save </t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_017</t>
+  </si>
+  <si>
+    <t>Verify whether a nurse is able add Intake Output details</t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursing Notes&gt;&gt;Intake Output Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select the start date and time of intake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start date and time should be selected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Intake Output details. Save </t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_018</t>
+  </si>
+  <si>
+    <t>Verify whether a nurse is able view previous Intake Output details</t>
+  </si>
+  <si>
+    <t>Click on "View Previous" to view the previous intake output details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous details should be displayed </t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_019</t>
+  </si>
+  <si>
+    <t>Verify whether a nurse can view Infusion/Transfusion details</t>
+  </si>
+  <si>
+    <t>Click on "View Previous" to view the previous Infusion/Transfusion details</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_016</t>
+  </si>
+  <si>
+    <t>Verify whether a nurse is able view previous Infusion/Transfusion entry from Intake Output details</t>
+  </si>
+  <si>
+    <t>Click on the Infusion/Transfusion Entry button</t>
+  </si>
+  <si>
+    <t>Infusion/Transfusion details should be displayed</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is create a special care request </t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursing Notes&gt;&gt;Physician Order Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intake Output Entry page should be displayed </t>
+  </si>
+  <si>
+    <t>Intake Output Entry should be entered and saved  successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physician Order Sheet should be displayed </t>
+  </si>
+  <si>
+    <t>Create the request with the following details
+Doctor
+Request Date
+Instruction
+Doctor's Remark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Care Request  should be created </t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_021</t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursig Admission Pedia&gt;&gt;System Review</t>
+  </si>
+  <si>
+    <t>Select the radio buttons and abnormal finding for each of the following 
+General
+Skin
+Eyes
+ENT
+Breast
+CVS/ Pulmonary
+GI
+GU
+Musculoskeletal
+Neuro/ Psych
+Endocrine
+Hem/Lymph
+Add details if any</t>
+  </si>
+  <si>
+    <t>Findings should be recorded</t>
+  </si>
+  <si>
+    <t>General
+Skin
+Eyes
+ENT
+Breast
+CVS/ Pulmonary
+GI
+GU
+Musculoskeletal
+Neuro/ Psych
+Endocrine</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is able to record more than one System Review for the patient </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is able to record System Review for the patient </t>
+  </si>
+  <si>
+    <t>Click on New and verify that the nurse can record a new findings</t>
+  </si>
+  <si>
+    <t>New finding should be recorded successfully</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is able to record and print System Review for the patient </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Print </t>
+  </si>
+  <si>
+    <t>User should be able to print</t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is able to add Admission Data </t>
+  </si>
+  <si>
+    <t>Navigate to Nursing Station&gt;&gt;Nursig Admission Pedia&gt;&gt;Admission Data- Pediatric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Review entry should be displayed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admission Data- Pediatric form should be displayed </t>
+  </si>
+  <si>
+    <t>Add details to the following section
+Admission Data
+Orientation To The Unit
+Patient Rights &amp; Responsibilities
+Valuables &amp; Equipment
+Medication History
+Sleep /Rest
+Psycho Social/ Economic Assessment 
+Growth &amp; Development
+Save the data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admission Data- Pediatric should be saved </t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is able to add more than one Admission Data </t>
+  </si>
+  <si>
+    <t>Click on New and add another Admission Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Admission Data- Pediatric should be saved </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether a nurse is able to add and pritn Admission Data </t>
+  </si>
+  <si>
+    <t>MED_NURS_TC_026</t>
   </si>
 </sst>
 </file>
@@ -482,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -571,6 +861,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -580,13 +873,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -720,7 +1013,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1767,7 +2060,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="10" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="10" customWidth="1"/>
@@ -1897,7 +2190,7 @@
       </c>
       <c r="B5" s="22">
         <f>'Nursing Station'!O2</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C5" s="22">
         <f>'Nursing Station'!O3</f>
@@ -1955,7 +2248,7 @@
       </c>
       <c r="B7" s="7">
         <f t="shared" ref="B7:G7" si="0">SUM(B2:B6)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
@@ -2016,16 +2309,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R732"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137:D140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="24" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="24" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="10" customWidth="1"/>
     <col min="6" max="6" width="48.140625" style="24" customWidth="1"/>
@@ -2074,14 +2367,14 @@
       <c r="L1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="Q1" s="31" t="s">
+      <c r="O1" s="31"/>
+      <c r="Q1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="31"/>
+      <c r="R1" s="32"/>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
@@ -2093,7 +2386,7 @@
       <c r="C2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="33" t="s">
         <v>57</v>
       </c>
       <c r="E2" s="10">
@@ -2115,7 +2408,7 @@
       </c>
       <c r="O2" s="21">
         <f>COUNTA(A:A)-1</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="11" t="s">
         <v>12</v>
@@ -2129,7 +2422,7 @@
       <c r="A3" s="35"/>
       <c r="B3" s="23"/>
       <c r="C3" s="17"/>
-      <c r="D3" s="33"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="10">
         <v>2</v>
       </c>
@@ -2163,7 +2456,7 @@
       <c r="A4" s="35"/>
       <c r="B4" s="23"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="33"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="10">
         <v>3</v>
       </c>
@@ -2193,7 +2486,7 @@
     <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="23"/>
-      <c r="D5" s="33"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="10">
         <v>4</v>
       </c>
@@ -2219,7 +2512,7 @@
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
       <c r="B6" s="23"/>
-      <c r="D6" s="33"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="10">
         <v>5</v>
       </c>
@@ -2238,7 +2531,7 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -2247,7 +2540,7 @@
       <c r="C8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="30" t="s">
         <v>58</v>
       </c>
       <c r="E8" s="10">
@@ -2263,9 +2556,9 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="23"/>
-      <c r="D9" s="33"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="10">
         <v>2</v>
       </c>
@@ -2279,9 +2572,9 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="23"/>
-      <c r="D10" s="33"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="10">
         <v>3</v>
       </c>
@@ -2298,9 +2591,9 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="23"/>
-      <c r="D11" s="33"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="10">
         <v>4</v>
       </c>
@@ -2331,7 +2624,7 @@
       <c r="C13" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="30" t="s">
         <v>56</v>
       </c>
       <c r="E13" s="10">
@@ -2348,7 +2641,7 @@
     </row>
     <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="23"/>
-      <c r="D14" s="33"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="10">
         <v>2</v>
       </c>
@@ -2363,7 +2656,7 @@
     </row>
     <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="23"/>
-      <c r="D15" s="33"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="10">
         <v>3</v>
       </c>
@@ -2378,7 +2671,7 @@
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="23"/>
-      <c r="D16" s="33"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="10">
         <v>3</v>
       </c>
@@ -2406,7 +2699,7 @@
       <c r="C18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="30" t="s">
         <v>59</v>
       </c>
       <c r="E18" s="10">
@@ -2423,7 +2716,7 @@
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="23"/>
-      <c r="D19" s="33"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="10">
         <v>2</v>
       </c>
@@ -2438,7 +2731,7 @@
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="23"/>
-      <c r="D20" s="33"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="10">
         <v>3</v>
       </c>
@@ -2453,7 +2746,7 @@
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="23"/>
-      <c r="D21" s="33"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="10">
         <v>4</v>
       </c>
@@ -2481,7 +2774,7 @@
       <c r="C23" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="30" t="s">
         <v>64</v>
       </c>
       <c r="E23" s="10">
@@ -2498,7 +2791,7 @@
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="23"/>
-      <c r="D24" s="33"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="10">
         <v>2</v>
       </c>
@@ -2513,7 +2806,7 @@
     </row>
     <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="23"/>
-      <c r="D25" s="33"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="10">
         <v>3</v>
       </c>
@@ -2528,7 +2821,7 @@
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="23"/>
-      <c r="D26" s="33"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="10">
         <v>4</v>
       </c>
@@ -2559,7 +2852,7 @@
       <c r="C28" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="30" t="s">
         <v>71</v>
       </c>
       <c r="E28" s="10">
@@ -2576,7 +2869,7 @@
     </row>
     <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="23"/>
-      <c r="D29" s="33"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="10">
         <v>2</v>
       </c>
@@ -2591,7 +2884,7 @@
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="23"/>
-      <c r="D30" s="33"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="10">
         <v>3</v>
       </c>
@@ -2606,7 +2899,7 @@
     </row>
     <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B31" s="23"/>
-      <c r="D31" s="33"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="10">
         <v>4</v>
       </c>
@@ -2637,7 +2930,7 @@
       <c r="C33" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="30" t="s">
         <v>76</v>
       </c>
       <c r="E33" s="10">
@@ -2654,7 +2947,7 @@
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="23"/>
-      <c r="D34" s="33"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="10">
         <v>2</v>
       </c>
@@ -2669,7 +2962,7 @@
     </row>
     <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="23"/>
-      <c r="D35" s="33"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="10">
         <v>3</v>
       </c>
@@ -2684,7 +2977,7 @@
     </row>
     <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B36" s="23"/>
-      <c r="D36" s="33"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="10">
         <v>4</v>
       </c>
@@ -2702,7 +2995,7 @@
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="23"/>
-      <c r="D37" s="33"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="10">
         <v>5</v>
       </c>
@@ -2717,7 +3010,7 @@
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="23"/>
-      <c r="D38" s="33"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="10">
         <v>6</v>
       </c>
@@ -2745,7 +3038,7 @@
       <c r="C40" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="30" t="s">
         <v>83</v>
       </c>
       <c r="E40" s="10">
@@ -2762,7 +3055,7 @@
     </row>
     <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="23"/>
-      <c r="D41" s="33"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="10">
         <v>2</v>
       </c>
@@ -2777,7 +3070,7 @@
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="23"/>
-      <c r="D42" s="33"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="10">
         <v>3</v>
       </c>
@@ -2792,7 +3085,7 @@
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
-      <c r="D43" s="33"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="10">
         <v>4</v>
       </c>
@@ -2807,7 +3100,7 @@
     </row>
     <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="23"/>
-      <c r="D44" s="33"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="10">
         <v>5</v>
       </c>
@@ -2838,7 +3131,7 @@
       <c r="C46" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="30" t="s">
         <v>91</v>
       </c>
       <c r="E46" s="10">
@@ -2855,7 +3148,7 @@
     </row>
     <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="23"/>
-      <c r="D47" s="33"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="10">
         <v>2</v>
       </c>
@@ -2870,7 +3163,7 @@
     </row>
     <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="23"/>
-      <c r="D48" s="33"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="10">
         <v>3</v>
       </c>
@@ -2885,7 +3178,7 @@
     </row>
     <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="23"/>
-      <c r="D49" s="33"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="10">
         <v>4</v>
       </c>
@@ -2900,7 +3193,7 @@
     </row>
     <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B50" s="23"/>
-      <c r="D50" s="33"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="10">
         <v>5</v>
       </c>
@@ -2918,7 +3211,7 @@
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="23"/>
-      <c r="D51" s="33"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="10">
         <v>6</v>
       </c>
@@ -2933,7 +3226,7 @@
     </row>
     <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="23"/>
-      <c r="D52" s="33"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="10">
         <v>7</v>
       </c>
@@ -2951,7 +3244,7 @@
       <c r="J53" s="17"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>96</v>
       </c>
@@ -2961,7 +3254,7 @@
       <c r="C54" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="30" t="s">
         <v>97</v>
       </c>
       <c r="E54" s="10">
@@ -2978,6 +3271,7 @@
     </row>
     <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="23"/>
+      <c r="D55" s="30"/>
       <c r="E55" s="10">
         <v>2</v>
       </c>
@@ -2992,6 +3286,7 @@
     </row>
     <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="23"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="10">
         <v>3</v>
       </c>
@@ -3009,6 +3304,7 @@
     </row>
     <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B57" s="23"/>
+      <c r="D57" s="30"/>
       <c r="E57" s="10">
         <v>4</v>
       </c>
@@ -3016,7 +3312,7 @@
         <v>100</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J57" s="17"/>
       <c r="K57" s="2"/>
@@ -3026,18 +3322,61 @@
       <c r="J58" s="17"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
+    <row r="59" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E59" s="10">
+        <v>1</v>
+      </c>
+      <c r="F59" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H59" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J59" s="17"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="23"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="10">
+        <v>2</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G60" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="J60" s="17"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B61" s="23"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="10">
+        <v>3</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G61" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="H61" s="24" t="s">
+        <v>108</v>
+      </c>
       <c r="J61" s="17"/>
       <c r="K61" s="2"/>
     </row>
@@ -3046,412 +3385,1229 @@
       <c r="J62" s="17"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
+    <row r="63" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" s="10">
+        <v>1</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J63" s="17"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="23"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="10">
+        <v>2</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="J64" s="17"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B65" s="23"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="10">
+        <v>3</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G65" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="H65" s="24" t="s">
+        <v>108</v>
+      </c>
       <c r="J65" s="17"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B66" s="23"/>
       <c r="J66" s="17"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="23"/>
+    <row r="67" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E67" s="10">
+        <v>1</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J67" s="17"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="23"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="10">
+        <v>2</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>116</v>
+      </c>
       <c r="J68" s="17"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="23"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="10">
+        <v>3</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>117</v>
+      </c>
       <c r="J69" s="17"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="23"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="10">
+        <v>4</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="J70" s="17"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B71" s="23"/>
       <c r="J71" s="17"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B72" s="23"/>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E72" s="10">
+        <v>1</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H72" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J72" s="17"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="23"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="10">
+        <v>2</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G73" s="24" t="s">
+        <v>128</v>
+      </c>
       <c r="J73" s="17"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="23"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="10">
+        <v>3</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G74" s="24" t="s">
+        <v>117</v>
+      </c>
       <c r="J74" s="17"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B75" s="23"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="10">
+        <v>4</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="G75" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="J75" s="17"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B76" s="23"/>
       <c r="J76" s="17"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" s="23"/>
+    <row r="77" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E77" s="10">
+        <v>1</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H77" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J77" s="17"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="23"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="10">
+        <v>2</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G78" s="24" t="s">
+        <v>129</v>
+      </c>
       <c r="J78" s="17"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="23"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="10">
+        <v>3</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="G79" s="24" t="s">
+        <v>131</v>
+      </c>
       <c r="J79" s="17"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B80" s="23"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="10">
+        <v>4</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H80" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="J80" s="17"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" s="23"/>
       <c r="J81" s="17"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" s="23"/>
+    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B82" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E82" s="10">
+        <v>1</v>
+      </c>
+      <c r="F82" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H82" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J82" s="17"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" s="23"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="10">
+        <v>2</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G83" s="24" t="s">
+        <v>129</v>
+      </c>
       <c r="J83" s="17"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="23"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="10">
+        <v>3</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="G84" s="24" t="s">
+        <v>131</v>
+      </c>
       <c r="J84" s="17"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B85" s="23"/>
+      <c r="D85" s="36"/>
+      <c r="E85" s="10">
+        <v>4</v>
+      </c>
+      <c r="F85" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="G85" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H85" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="J85" s="17"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B86" s="23"/>
       <c r="J86" s="17"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="23"/>
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B87" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E87" s="10">
+        <v>1</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H87" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J87" s="17"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="23"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="10">
+        <v>2</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G88" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="J88" s="17"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="23"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="10">
+        <v>3</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G89" s="24" t="s">
+        <v>139</v>
+      </c>
       <c r="J89" s="17"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B90" s="23"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="10">
+        <v>4</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G90" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H90" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="J90" s="17"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B91" s="23"/>
       <c r="J91" s="17"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" s="23"/>
+    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E92" s="10">
+        <v>1</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H92" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J92" s="17"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B93" s="23"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="10">
+        <v>2</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G93" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="J93" s="17"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B94" s="23"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="10">
+        <v>3</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G94" s="24" t="s">
+        <v>139</v>
+      </c>
       <c r="J94" s="17"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="23"/>
+      <c r="D95" s="30"/>
+      <c r="E95" s="10">
+        <v>4</v>
+      </c>
+      <c r="F95" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G95" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H95" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="J95" s="17"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="23"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="10">
+        <v>5</v>
+      </c>
+      <c r="F96" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G96" s="24" t="s">
+        <v>144</v>
+      </c>
       <c r="J96" s="17"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B97" s="23"/>
       <c r="J97" s="17"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B98" s="23"/>
+    <row r="98" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B98" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E98" s="10">
+        <v>1</v>
+      </c>
+      <c r="F98" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H98" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J98" s="17"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="23"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="10">
+        <v>2</v>
+      </c>
+      <c r="F99" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="J99" s="17"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B100" s="23"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="10">
+        <v>3</v>
+      </c>
+      <c r="F100" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G100" s="24" t="s">
+        <v>139</v>
+      </c>
       <c r="J100" s="17"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B101" s="23"/>
+      <c r="D101" s="30"/>
+      <c r="E101" s="10">
+        <v>4</v>
+      </c>
+      <c r="F101" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G101" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H101" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="J101" s="17"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="23"/>
+      <c r="D102" s="30"/>
+      <c r="E102" s="10">
+        <v>5</v>
+      </c>
+      <c r="F102" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G102" s="24" t="s">
+        <v>144</v>
+      </c>
       <c r="J102" s="17"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B103" s="23"/>
       <c r="J103" s="17"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="23"/>
+    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B104" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E104" s="10">
+        <v>1</v>
+      </c>
+      <c r="F104" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H104" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J104" s="17"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="23"/>
+      <c r="D105" s="30"/>
+      <c r="E105" s="10">
+        <v>2</v>
+      </c>
+      <c r="F105" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G105" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="J105" s="17"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B106" s="23"/>
+      <c r="D106" s="30"/>
+      <c r="E106" s="10">
+        <v>3</v>
+      </c>
+      <c r="F106" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G106" s="24" t="s">
+        <v>139</v>
+      </c>
       <c r="J106" s="17"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B107" s="23"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="10">
+        <v>4</v>
+      </c>
+      <c r="F107" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G107" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H107" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="J107" s="17"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="23"/>
+      <c r="D108" s="30"/>
+      <c r="E108" s="10">
+        <v>5</v>
+      </c>
+      <c r="F108" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="G108" s="24" t="s">
+        <v>151</v>
+      </c>
       <c r="J108" s="17"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B109" s="23"/>
       <c r="J109" s="17"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B110" s="23"/>
+    <row r="110" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B110" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E110" s="10">
+        <v>1</v>
+      </c>
+      <c r="F110" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H110" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J110" s="17"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="23"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="10">
+        <v>2</v>
+      </c>
+      <c r="F111" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="G111" s="24" t="s">
+        <v>157</v>
+      </c>
       <c r="J111" s="17"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B112" s="23"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="10">
+        <v>3</v>
+      </c>
+      <c r="F112" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G112" s="24" t="s">
+        <v>159</v>
+      </c>
       <c r="J112" s="17"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B113" s="23"/>
       <c r="J113" s="17"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B114" s="23"/>
+    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B114" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="E114" s="10">
+        <v>1</v>
+      </c>
+      <c r="F114" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H114" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J114" s="17"/>
       <c r="K114" s="2"/>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="23"/>
+      <c r="D115" s="30"/>
+      <c r="E115" s="10">
+        <v>2</v>
+      </c>
+      <c r="F115" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="G115" s="24" t="s">
+        <v>177</v>
+      </c>
       <c r="J115" s="17"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="B116" s="23"/>
+      <c r="D116" s="30"/>
+      <c r="E116" s="10">
+        <v>3</v>
+      </c>
+      <c r="F116" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="G116" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="H116" s="24" t="s">
+        <v>164</v>
+      </c>
       <c r="J116" s="17"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B117" s="23"/>
       <c r="J117" s="17"/>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B118" s="23"/>
+    <row r="118" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="B118" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="E118" s="10">
+        <v>1</v>
+      </c>
+      <c r="F118" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H118" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J118" s="17"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B119" s="23"/>
+      <c r="D119" s="30"/>
+      <c r="E119" s="10">
+        <v>2</v>
+      </c>
+      <c r="F119" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="G119" s="24" t="s">
+        <v>177</v>
+      </c>
       <c r="J119" s="17"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="B120" s="23"/>
+      <c r="D120" s="30"/>
+      <c r="E120" s="10">
+        <v>3</v>
+      </c>
+      <c r="F120" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="G120" s="24" t="s">
+        <v>163</v>
+      </c>
       <c r="J120" s="17"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B121" s="23"/>
+      <c r="D121" s="30"/>
+      <c r="E121" s="10">
+        <v>4</v>
+      </c>
+      <c r="F121" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G121" s="24" t="s">
+        <v>169</v>
+      </c>
       <c r="J121" s="17"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B122" s="23"/>
       <c r="J122" s="17"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B123" s="23"/>
+    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B123" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D123" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E123" s="10">
+        <v>1</v>
+      </c>
+      <c r="F123" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H123" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J123" s="17"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B124" s="23"/>
+      <c r="D124" s="30"/>
+      <c r="E124" s="10">
+        <v>2</v>
+      </c>
+      <c r="F124" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="G124" s="24" t="s">
+        <v>177</v>
+      </c>
       <c r="J124" s="17"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="B125" s="23"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="10">
+        <v>3</v>
+      </c>
+      <c r="F125" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="G125" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="H125" s="24" t="s">
+        <v>164</v>
+      </c>
       <c r="J125" s="17"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="23"/>
+      <c r="D126" s="30"/>
+      <c r="E126" s="10">
+        <v>4</v>
+      </c>
+      <c r="F126" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="G126" s="24" t="s">
+        <v>173</v>
+      </c>
       <c r="J126" s="17"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B127" s="23"/>
       <c r="J127" s="17"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B128" s="23"/>
+    <row r="128" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B128" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="E128" s="10">
+        <v>1</v>
+      </c>
+      <c r="F128" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H128" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J128" s="17"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B129" s="23"/>
+      <c r="D129" s="30"/>
+      <c r="E129" s="10">
+        <v>2</v>
+      </c>
+      <c r="F129" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G129" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="J129" s="17"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="B130" s="23"/>
+      <c r="D130" s="30"/>
+      <c r="E130" s="10">
+        <v>3</v>
+      </c>
+      <c r="F130" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="G130" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="J130" s="17"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B131" s="23"/>
       <c r="J131" s="17"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B132" s="23"/>
+    <row r="132" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B132" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C132" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D132" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E132" s="10">
+        <v>1</v>
+      </c>
+      <c r="F132" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H132" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J132" s="17"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B133" s="23"/>
+      <c r="D133" s="30"/>
+      <c r="E133" s="10">
+        <v>2</v>
+      </c>
+      <c r="F133" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G133" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="J133" s="17"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="B134" s="23"/>
+      <c r="D134" s="30"/>
+      <c r="E134" s="10">
+        <v>3</v>
+      </c>
+      <c r="F134" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="G134" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="J134" s="17"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="23"/>
+      <c r="D135" s="30"/>
+      <c r="E135" s="10">
+        <v>4</v>
+      </c>
+      <c r="F135" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="G135" s="24" t="s">
+        <v>184</v>
+      </c>
       <c r="J135" s="17"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B136" s="23"/>
       <c r="J136" s="17"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B137" s="23"/>
+    <row r="137" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B137" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C137" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E137" s="10">
+        <v>1</v>
+      </c>
+      <c r="F137" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H137" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="J137" s="17"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B138" s="23"/>
+      <c r="D138" s="30"/>
+      <c r="E138" s="10">
+        <v>2</v>
+      </c>
+      <c r="F138" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G138" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="J138" s="17"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="B139" s="23"/>
+      <c r="D139" s="30"/>
+      <c r="E139" s="10">
+        <v>3</v>
+      </c>
+      <c r="F139" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="G139" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="J139" s="17"/>
       <c r="K139" s="2"/>
     </row>
-    <row r="140" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B140" s="23"/>
+      <c r="D140" s="30"/>
+      <c r="E140" s="10">
+        <v>4</v>
+      </c>
+      <c r="F140" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="G140" s="24" t="s">
+        <v>173</v>
+      </c>
       <c r="J140" s="17"/>
       <c r="K140" s="2"/>
     </row>
-    <row r="141" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B141" s="23"/>
       <c r="J141" s="17"/>
       <c r="K141" s="2"/>
     </row>
-    <row r="142" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B142" s="23"/>
       <c r="J142" s="17"/>
       <c r="K142" s="2"/>
     </row>
-    <row r="143" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B143" s="23"/>
       <c r="J143" s="17"/>
       <c r="K143" s="2"/>
     </row>
-    <row r="144" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B144" s="23"/>
       <c r="J144" s="17"/>
       <c r="K144" s="2"/>
@@ -6228,7 +7384,19 @@
       <c r="K732" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="31">
+    <mergeCell ref="D128:D130"/>
+    <mergeCell ref="D123:D126"/>
+    <mergeCell ref="D132:D135"/>
+    <mergeCell ref="D137:D140"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="D114:D116"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="D92:D96"/>
+    <mergeCell ref="D98:D102"/>
     <mergeCell ref="D46:D52"/>
     <mergeCell ref="D40:D44"/>
     <mergeCell ref="D13:D16"/>
@@ -6242,6 +7410,12 @@
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A2:A6"/>
+    <mergeCell ref="D77:D80"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="D72:D75"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J485:J687" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -6250,13 +7424,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K732" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B608" xr:uid="{9C290696-F92B-4C43-BEFE-658BF68D334E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B608" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"CAS/ Appointment, Out Patient, Care Desk, EMR, Lab &amp; General Billing, Pharmacy Billing, Lab Results, Radiology, Insurance Desk, Casualty, MRD, In Patient, Nursing Station, Theatre, Indent, Store Management"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C659:C728" xr:uid="{E0298947-6D09-423C-8721-8EAB39CE165E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C659:C728" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Nithya VS, Poonima John, Prapancha, Preethi Pathrose, Parvathy P, Semin Das, Sangeetha, Rijo J Patric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J484 C2:C658" xr:uid="{3D2B8E7F-289D-450A-9428-89381A0B654F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J484 C2:C658" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"Nithya VS, Poonima John, Prapancha, Preethi Pathrose, Semin Das, Sangeetha, Rijo J Patric"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>